<commit_message>
Aula 03 de Junho
</commit_message>
<xml_diff>
--- a/Pasta1.xlsx
+++ b/Pasta1.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="ClienteServidor" sheetId="1" r:id="rId1"/>
+    <sheet name="DOM" sheetId="2" r:id="rId2"/>
+    <sheet name="Tables" sheetId="3" r:id="rId3"/>
+    <sheet name="Layouts" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>HTML</t>
   </si>
@@ -78,12 +79,30 @@
   <si>
     <t>T</t>
   </si>
+  <si>
+    <t>HEADER</t>
+  </si>
+  <si>
+    <t>MENU</t>
+  </si>
+  <si>
+    <t>BARRA DE NAVEGAÇÃO</t>
+  </si>
+  <si>
+    <t>CONTEÚDO</t>
+  </si>
+  <si>
+    <t>ADDS</t>
+  </si>
+  <si>
+    <t>RODAPÉ</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,8 +110,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +129,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -146,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -158,6 +215,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2791,7 +2867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -2806,46 +2882,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G8" s="2"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="2"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="I9" s="2"/>
+      <c r="I9" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2856,4 +2932,163 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C2:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:C15"/>
+    <mergeCell ref="D5:G15"/>
+    <mergeCell ref="H5:H15"/>
+    <mergeCell ref="C16:H16"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>